<commit_message>
Update program procedure to reflect new v2.1 language.
</commit_message>
<xml_diff>
--- a/onc_certification_g10_matrix.xlsx
+++ b/onc_certification_g10_matrix.xlsx
@@ -12153,32 +12153,24 @@
       </c>
       <c r="J25" s="158"/>
     </row>
-    <row r="26" spans="3:10" s="157" customFormat="1" ht="100" customHeight="1">
+    <row r="26" spans="3:10" s="157" customFormat="1" ht="60" customHeight="1">
       <c r="C26" s="157" t="str">
         <v xml:space="preserve">AUTH-PATIENT-13 </v>
       </c>
       <c r="D26" s="158" t="str">
-        <v xml:space="preserve">[Both] The health IT developer demonstrates the ability of
-the Health IT Module to return an error response if the following
-parameters provided by an application to the Health IT Module in
-step 8 of this section do not match the parameters originally
-provided to an application by the Health IT Module in step 2 of
-this section according to the implementation specification
-adopted in § 170.215(a)(3):
-* “launch”; and
-* “aud”.
+        <v xml:space="preserve">[Both] The health IT developer demonstrates the ability of the Health
+IT Module to return an error response if the "aud" parameter provided
+by an application to the Health IT Module in Step 8, is not a valid
+FHIR® resource server associated with the Health IT Module's
+authorization server. 
 </v>
       </c>
       <c r="E26" s="158" t="str">
-        <v xml:space="preserve">[Both] The tester verifies the ability of the Health IT
-Module to return an error response if the following parameters
-provided by an application to the Health IT Module in step 8 of
-this section do not match the parameters originally provided to an
-application by the Health IT Module in step 2 of this section
-according to the implementation specification adopted in §
-170.215(a)(3):
-* “launch”; and
-* “aud”.
+        <v xml:space="preserve">[Both] The tester verifies the ability of the Health IT Module to
+return an error response if the "aud" parameter provided by an
+application to the Health IT Module in Step 8, is not a valid FHIR®
+resource server associated with the Health IT Module's authorization
+server.
 </v>
       </c>
       <c r="F26" s="157" t="str">

</xml_diff>

<commit_message>
Update test procedure mapping matrix.
</commit_message>
<xml_diff>
--- a/onc_certification_g10_matrix.xlsx
+++ b/onc_certification_g10_matrix.xlsx
@@ -1596,7 +1596,7 @@
   <sheetData>
     <row r="1" spans="2:2" s="3" customFormat="1" ht="20" customHeight="1">
       <c r="B1" s="3" t="str">
-        <v>ONC Certification (g)(10) Test Kit (v2.2.2)</v>
+        <v>ONC Certification (g)(10) Test Kit (v2.3.0)</v>
       </c>
     </row>
     <row r="2" spans="3:58" s="3" customFormat="1" ht="20" customHeight="1">
@@ -1759,7 +1759,7 @@
         <v>5.1 Bulk Data Authorization</v>
       </c>
       <c r="AU3" s="17" t="str">
-        <v>5.2 Group Compartment Export Tests</v>
+        <v>5.2 Group Compartment Export Tests STU1</v>
       </c>
       <c r="AV3" s="17" t="str">
         <v>5.3 Group Compartment Export Validation Tests</v>
@@ -21991,7 +21991,7 @@
     </row>
     <row r="367" spans="2:2" customFormat="false">
       <c r="B367" s="0" t="str">
-        <v>5.2: Group Compartment Export Tests</v>
+        <v>5.2: Group Compartment Export Tests STU1</v>
       </c>
     </row>
     <row r="368" spans="1:6" s="157" customFormat="1" ht="60" customHeight="1">

</xml_diff>

<commit_message>
Regenerated matrix after test name change.
</commit_message>
<xml_diff>
--- a/onc_certification_g10_matrix.xlsx
+++ b/onc_certification_g10_matrix.xlsx
@@ -1759,7 +1759,7 @@
         <v>5.1 Bulk Data Authorization</v>
       </c>
       <c r="AU3" s="17" t="str">
-        <v>5.2 Group Compartment Export Tests STU1</v>
+        <v>5.2 Group Compartment Export Tests</v>
       </c>
       <c r="AV3" s="17" t="str">
         <v>5.3 Group Compartment Export Validation Tests</v>
@@ -21991,7 +21991,7 @@
     </row>
     <row r="367" spans="2:2" customFormat="false">
       <c r="B367" s="0" t="str">
-        <v>5.2: Group Compartment Export Tests STU1</v>
+        <v>5.2: Group Compartment Export Tests</v>
       </c>
     </row>
     <row r="368" spans="1:6" s="157" customFormat="1" ht="60" customHeight="1">

</xml_diff>

<commit_message>
FI-1705: Add public url attestation (#266)
* add attestation for public urls

* update matrix metadata

* regenerate matrix

* Update lib/onc_certification_g10_test_kit/visual_inspection_and_attestations_group.rb

Co-authored-by: Rob Scanlon <robscanlon@gmail.com>

Co-authored-by: Rob Scanlon <robscanlon@gmail.com>
</commit_message>
<xml_diff>
--- a/onc_certification_g10_matrix.xlsx
+++ b/onc_certification_g10_matrix.xlsx
@@ -34129,11 +34129,11 @@
       <c r="EK74" s="1" t="str">
         <v/>
       </c>
-      <c r="EL74" s="346" t="str">
+      <c r="EL74" s="345" t="str">
         <v/>
       </c>
       <c r="EN74" s="1" t="str">
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
   </sheetData>
@@ -37008,10 +37008,10 @@
         <v/>
       </c>
       <c r="G103" s="350" t="str">
-        <v>no</v>
+        <v>yes</v>
       </c>
       <c r="H103" s="351" t="str">
-        <v/>
+        <v>9.10.14</v>
       </c>
       <c r="I103" s="351"/>
       <c r="J103" s="351"/>
@@ -37022,7 +37022,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mv="urn:schemas-microsoft-com:mac:vml">
-  <dimension ref="A1:F1195"/>
+  <dimension ref="A1:F1196"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="3.7109375" customWidth="1"/>
@@ -64062,6 +64062,28 @@
         <v>AUT-PAT-21</v>
       </c>
     </row>
+    <row r="1196" spans="1:6" s="350" customFormat="1" ht="40" customHeight="1">
+      <c r="A1196" s="351" t="str">
+        <v/>
+      </c>
+      <c r="B1196" s="351" t="str">
+        <v/>
+      </c>
+      <c r="C1196" s="351" t="str">
+        <v>9.10.14</v>
+      </c>
+      <c r="D1196" s="351" t="str">
+        <v>Health IT developer demonstrates the public location of its base URLs</v>
+      </c>
+      <c r="E1196" s="351" t="str">
+        <v xml:space="preserve">To fulfill the API Maintenance of Certification requirement at §
+170.404(b)(2), the health IT developer demonstrates the public location
+of its certified API technology service base URLs.</v>
+      </c>
+      <c r="F1196" s="351" t="str">
+        <v>API-DOC-3</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>